<commit_message>
57 - ERD maken ( https://italent.cloudapp.net:9443/ccm/web/projects/iTalent#action=com.ibm.team.workitem.viewWorkItem&id=57 )
</commit_message>
<xml_diff>
--- a/italent/documents/analyse/ClassDiagram/EntityDraft.xlsx
+++ b/italent/documents/analyse/ClassDiagram/EntityDraft.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkspaceITalent\italent\documents\analyse\use-cases\EntityRelationDiagram\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkspaceITalent\italent\documents\analyse\ClassDiagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
   <si>
     <t>Users</t>
   </si>
@@ -172,6 +172,15 @@
   </si>
   <si>
     <t>WantedSubscribers</t>
+  </si>
+  <si>
+    <t>DepartmentId</t>
+  </si>
+  <si>
+    <t>isPublic</t>
+  </si>
+  <si>
+    <t>aantal</t>
   </si>
 </sst>
 </file>
@@ -542,7 +551,7 @@
   <dimension ref="L4:U24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,7 +680,7 @@
         <v>13</v>
       </c>
       <c r="U7" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="12:21" x14ac:dyDescent="0.25">
@@ -681,6 +690,9 @@
       <c r="Q8" t="s">
         <v>21</v>
       </c>
+      <c r="U8" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="12:21" x14ac:dyDescent="0.25">
       <c r="Q9" t="s">
@@ -705,6 +717,11 @@
     <row r="13" spans="12:21" x14ac:dyDescent="0.25">
       <c r="Q13" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="Q14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="12:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
58 - Use case diagram studenten ( https://italent.cloudapp.net:9443/ccm/web/projects/iTalent#action=com.ibm.team.workitem.viewWorkItem&id=58 )
</commit_message>
<xml_diff>
--- a/italent/documents/analyse/ClassDiagram/EntityDraft.xlsx
+++ b/italent/documents/analyse/ClassDiagram/EntityDraft.xlsx
@@ -29,7 +29,7 @@
     <author>NVD</author>
   </authors>
   <commentList>
-    <comment ref="Q13" authorId="0" shapeId="0">
+    <comment ref="F13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -548,275 +548,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="L4:U24"/>
+  <dimension ref="A4:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.42578125" customWidth="1"/>
-    <col min="15" max="20" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13" customWidth="1"/>
-    <col min="22" max="22" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="12:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="L4" s="1" t="s">
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="12:21" x14ac:dyDescent="0.25">
-      <c r="L5" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="M5" t="s">
+      <c r="B5" t="s">
         <v>34</v>
       </c>
-      <c r="N5" t="s">
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="O5" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="P5" t="s">
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="R5" t="s">
+      <c r="G5" t="s">
         <v>12</v>
       </c>
-      <c r="S5" t="s">
+      <c r="H5" t="s">
         <v>9</v>
       </c>
-      <c r="T5" t="s">
+      <c r="I5" t="s">
         <v>25</v>
       </c>
-      <c r="U5" t="s">
+      <c r="J5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="12:21" x14ac:dyDescent="0.25">
-      <c r="L6" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="M6" t="s">
+      <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="N6" t="s">
+      <c r="C6" t="s">
         <v>34</v>
       </c>
-      <c r="O6" t="s">
+      <c r="D6" t="s">
         <v>11</v>
       </c>
-      <c r="P6" t="s">
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="F6" t="s">
         <v>36</v>
       </c>
-      <c r="R6" t="s">
+      <c r="G6" t="s">
         <v>13</v>
       </c>
-      <c r="S6" t="s">
+      <c r="H6" t="s">
         <v>24</v>
       </c>
-      <c r="T6" t="s">
+      <c r="I6" t="s">
         <v>11</v>
       </c>
-      <c r="U6" t="s">
+      <c r="J6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="12:21" x14ac:dyDescent="0.25">
-      <c r="L7" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="O7" t="s">
+      <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="P7" t="s">
+      <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="F7" t="s">
         <v>9</v>
       </c>
-      <c r="R7" t="s">
+      <c r="G7" t="s">
         <v>11</v>
       </c>
-      <c r="T7" t="s">
+      <c r="I7" t="s">
         <v>13</v>
       </c>
-      <c r="U7" t="s">
+      <c r="J7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="12:21" x14ac:dyDescent="0.25">
-      <c r="L8" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="F8" t="s">
         <v>21</v>
       </c>
-      <c r="U8" t="s">
+      <c r="J8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="12:21" x14ac:dyDescent="0.25">
-      <c r="Q9" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="12:21" x14ac:dyDescent="0.25">
-      <c r="Q10" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="12:21" x14ac:dyDescent="0.25">
-      <c r="Q11" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="12:21" x14ac:dyDescent="0.25">
-      <c r="Q12" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="12:21" x14ac:dyDescent="0.25">
-      <c r="Q13" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="12:21" x14ac:dyDescent="0.25">
-      <c r="Q14" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="12:21" x14ac:dyDescent="0.25">
-      <c r="L22" t="s">
-        <v>29</v>
-      </c>
-      <c r="M22" t="s">
-        <v>29</v>
-      </c>
-      <c r="N22" t="s">
-        <v>29</v>
-      </c>
-      <c r="O22" t="s">
-        <v>29</v>
-      </c>
-      <c r="P22" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>29</v>
-      </c>
-      <c r="R22" t="s">
-        <v>29</v>
-      </c>
-      <c r="S22" t="s">
-        <v>29</v>
-      </c>
-      <c r="T22" t="s">
-        <v>29</v>
-      </c>
-      <c r="U22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="12:21" x14ac:dyDescent="0.25">
-      <c r="L23" t="s">
-        <v>30</v>
-      </c>
-      <c r="M23" t="s">
-        <v>30</v>
-      </c>
-      <c r="N23" t="s">
-        <v>30</v>
-      </c>
-      <c r="O23" t="s">
-        <v>30</v>
-      </c>
-      <c r="P23" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>30</v>
-      </c>
-      <c r="R23" t="s">
-        <v>30</v>
-      </c>
-      <c r="S23" t="s">
-        <v>30</v>
-      </c>
-      <c r="T23" t="s">
-        <v>30</v>
-      </c>
-      <c r="U23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="12:21" x14ac:dyDescent="0.25">
-      <c r="L24" t="s">
-        <v>31</v>
-      </c>
-      <c r="M24" t="s">
-        <v>31</v>
-      </c>
-      <c r="N24" t="s">
-        <v>31</v>
-      </c>
-      <c r="O24" t="s">
-        <v>31</v>
-      </c>
-      <c r="P24" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>31</v>
-      </c>
-      <c r="R24" t="s">
-        <v>31</v>
-      </c>
-      <c r="S24" t="s">
-        <v>31</v>
-      </c>
-      <c r="T24" t="s">
-        <v>31</v>
-      </c>
-      <c r="U24" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" t="s">
+        <v>30</v>
+      </c>
+      <c r="J23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" t="s">
+        <v>31</v>
+      </c>
+      <c r="J24" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>